<commit_message>
Adding powerBi file copleted
</commit_message>
<xml_diff>
--- a/AdventureWorksDW2022_data/Data/Budget.xlsx
+++ b/AdventureWorksDW2022_data/Data/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/56307aa289e10451/Pulpit/Github/PowerBI/AdventureWorksDW2022_data/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAC2FF6D-CCC5-41FF-93FC-69ED15102AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{EAC2FF6D-CCC5-41FF-93FC-69ED15102AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE7E1D77-2AC3-43D8-B2F3-B9DF07EDBD15}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{1D5C6C17-7EF3-4565-B1D7-CB87B9CB41A6}"/>
   </bookViews>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3227B1-4145-4785-B64B-D5C2B4F08A4E}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B29"/>
+      <selection activeCell="B1" sqref="B1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -417,258 +417,411 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1">
-        <v>44562</v>
+        <v>44044</v>
       </c>
       <c r="B1">
-        <v>800000</v>
+        <f>B18+(-1)^(B18/100000)*200000</f>
+        <v>1000000</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
-        <v>44593</v>
+        <v>44075</v>
       </c>
       <c r="B2">
-        <v>900000</v>
+        <f t="shared" ref="B2:B17" si="0">B19+(-1)^(B19/100000)*200000</f>
+        <v>700000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
-        <v>44621</v>
+        <v>44105</v>
       </c>
       <c r="B3">
-        <v>1000000</v>
+        <f t="shared" si="0"/>
+        <v>1200000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
-        <v>44652</v>
+        <v>44136</v>
       </c>
       <c r="B4">
-        <v>1200000</v>
+        <f t="shared" si="0"/>
+        <v>1400000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
-        <v>44682</v>
+        <v>44166</v>
       </c>
       <c r="B5">
-        <v>1100000</v>
+        <f t="shared" si="0"/>
+        <v>900000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
-        <v>44713</v>
+        <v>44197</v>
       </c>
       <c r="B6">
-        <v>1200000</v>
+        <f t="shared" si="0"/>
+        <v>1400000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
-        <v>44743</v>
+        <v>44228</v>
       </c>
       <c r="B7">
-        <v>1000000</v>
+        <f t="shared" si="0"/>
+        <v>1200000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
-        <v>44774</v>
+        <v>44256</v>
       </c>
       <c r="B8">
-        <v>1000000</v>
+        <f t="shared" si="0"/>
+        <v>1200000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
-        <v>44805</v>
+        <v>44287</v>
       </c>
       <c r="B9">
-        <v>1200000</v>
+        <f t="shared" si="0"/>
+        <v>1400000</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
-        <v>44835</v>
+        <v>44317</v>
       </c>
       <c r="B10">
-        <v>1200000</v>
+        <f t="shared" si="0"/>
+        <v>1400000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
-        <v>44866</v>
+        <v>44348</v>
       </c>
       <c r="B11">
-        <v>1400000</v>
+        <f t="shared" si="0"/>
+        <v>1600000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
-        <v>44896</v>
+        <v>44378</v>
       </c>
       <c r="B12">
-        <v>1500000</v>
+        <f t="shared" si="0"/>
+        <v>1300000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
-        <v>44927</v>
+        <v>44409</v>
       </c>
       <c r="B13">
-        <f>B1+100000</f>
-        <v>900000</v>
+        <f t="shared" si="0"/>
+        <v>700000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
-        <v>44958</v>
+        <v>44440</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:B29" si="0">B2+100000</f>
-        <v>1000000</v>
+        <f t="shared" si="0"/>
+        <v>1200000</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
-        <v>44986</v>
+        <v>44470</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>1100000</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
-        <v>45017</v>
+        <v>44501</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>1300000</v>
+        <v>1100000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
-        <v>45047</v>
+        <v>44531</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>1200000</v>
+        <v>1400000</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
-        <v>45078</v>
+        <v>44562</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
-        <v>1300000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
-        <v>45108</v>
+        <v>44593</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
-        <v>1100000</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
-        <v>45139</v>
+        <v>44621</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
-        <v>1100000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
-        <v>45170</v>
+        <v>44652</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
-        <v>1300000</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
-        <v>45200</v>
+        <v>44682</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
-        <v>1300000</v>
+        <v>1100000</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
-        <v>45231</v>
+        <v>44713</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
-        <v>1500000</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
-        <v>45261</v>
+        <v>44743</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
-        <v>1600000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
-        <v>45292</v>
+        <v>44774</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
-        <v>45323</v>
+        <v>44805</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
-        <v>1100000</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
-        <v>45352</v>
+        <v>44835</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
         <v>1200000</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
-        <v>45383</v>
+        <v>44866</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
         <v>1400000</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
-        <v>45413</v>
+        <v>44896</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
-        <v>1300000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
+        <v>44927</v>
+      </c>
+      <c r="B30">
+        <f>B18+100000</f>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
+        <v>44958</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ref="B31:B46" si="1">B19+100000</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
+        <v>44986</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
+        <v>45017</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="1">
+        <v>45108</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" s="1">
+        <v>45139</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="1"/>
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" s="1">
+        <v>45170</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="1"/>
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="1"/>
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A40" s="1">
+        <v>45231</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41" s="1">
+        <v>45261</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="1"/>
+        <v>1600000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42" s="1">
+        <v>45292</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43" s="1">
+        <v>45323</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="1"/>
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44" s="1">
+        <v>45352</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="1"/>
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="1"/>
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46" s="1">
+        <v>45413</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="1"/>
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47" s="1">
         <v>45444</v>
       </c>
-      <c r="B30">
+      <c r="B47">
         <v>900000</v>
       </c>
     </row>

</xml_diff>